<commit_message>
Ajuste de producto realizado
Pendiente de %
</commit_message>
<xml_diff>
--- a/Nomina/Info.xlsx
+++ b/Nomina/Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Documents\GitHub\Problem_Set_1\ForeverChic\Nomina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9A04CE-8979-4403-9789-870B09554744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AEA4EC-6490-4C7F-9311-3E6E0A0F975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{E10BBF24-8B64-47E0-9392-E6A1EA239C1A}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="97">
   <si>
     <t>Alianzas de Marketing</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Ivonne Mancipe</t>
+  </si>
+  <si>
+    <t>Ines torres</t>
   </si>
 </sst>
 </file>
@@ -1079,8 +1082,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A17379-BA46-4212-9EC9-9D0965690188}" name="Tabla1" displayName="Tabla1" ref="A1:A15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:A15" xr:uid="{D8A17379-BA46-4212-9EC9-9D0965690188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A17379-BA46-4212-9EC9-9D0965690188}" name="Tabla1" displayName="Tabla1" ref="A1:A16" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:A16" xr:uid="{D8A17379-BA46-4212-9EC9-9D0965690188}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DDDF52DE-A7F5-4918-BAE0-228DFC5015C3}" name="Profesional" dataDxfId="21"/>
   </tableColumns>
@@ -3945,11 +3948,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB14EE81-1336-48D1-AF56-B5F648183D15}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4030,6 +4031,11 @@
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>